<commit_message>
added 304 Dholuo from Lolwe tv, rlv and ramogi twitter
</commit_message>
<xml_diff>
--- a/To be translated.xlsx
+++ b/To be translated.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ogayo\OneDrive\Desktop\Masakhane\Luo-News-Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA822EFE-4FBC-4971-8B4D-D9D373C19579}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7B1E5DB-91B0-4D4A-886D-A1B0D463F76E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9198,8 +9198,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9709E34-8E42-4397-B876-0C6E97F59BCE}">
   <dimension ref="A1:B1134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1118" workbookViewId="0">
-      <selection activeCell="B1133" sqref="B1133"/>
+    <sheetView tabSelected="1" topLeftCell="A1132" workbookViewId="0">
+      <selection activeCell="B1139" sqref="B1139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9296,7 +9296,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="34.200000000000003" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>434</v>
       </c>
@@ -9320,7 +9320,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>437</v>
       </c>
@@ -9328,7 +9328,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" ht="34.200000000000003" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>438</v>
       </c>
@@ -9336,7 +9336,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>439</v>
       </c>
@@ -9344,7 +9344,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>440</v>
       </c>
@@ -9784,7 +9784,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="7" t="s">
         <v>494</v>
       </c>
@@ -9928,7 +9928,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" s="7" t="s">
         <v>511</v>
       </c>
@@ -10008,7 +10008,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="101" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" s="7" t="s">
         <v>527</v>
       </c>
@@ -10040,7 +10040,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="105" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" s="7" t="s">
         <v>529</v>
       </c>
@@ -10200,7 +10200,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="125" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" s="7" t="s">
         <v>1500</v>
       </c>
@@ -10264,7 +10264,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="133" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133" s="7" t="s">
         <v>550</v>
       </c>
@@ -10336,7 +10336,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="142" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A142" s="7" t="s">
         <v>560</v>
       </c>
@@ -10384,7 +10384,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="148" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:2" ht="34.200000000000003" x14ac:dyDescent="0.3">
       <c r="A148" s="7" t="s">
         <v>567</v>
       </c>
@@ -10416,7 +10416,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="152" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A152" s="7" t="s">
         <v>571</v>
       </c>
@@ -10432,7 +10432,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="154" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A154" s="7" t="s">
         <v>573</v>
       </c>
@@ -10440,7 +10440,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="155" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A155" s="7" t="s">
         <v>574</v>
       </c>
@@ -10448,7 +10448,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="156" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A156" s="7" t="s">
         <v>575</v>
       </c>
@@ -10464,7 +10464,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="158" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A158" s="7" t="s">
         <v>577</v>
       </c>
@@ -10472,7 +10472,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="159" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:2" ht="34.200000000000003" x14ac:dyDescent="0.3">
       <c r="A159" s="7" t="s">
         <v>578</v>
       </c>
@@ -10480,7 +10480,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="160" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A160" s="7" t="s">
         <v>579</v>
       </c>
@@ -10496,7 +10496,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="162" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:2" ht="34.200000000000003" x14ac:dyDescent="0.3">
       <c r="A162" s="7" t="s">
         <v>580</v>
       </c>
@@ -10536,7 +10536,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="167" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:2" ht="34.200000000000003" x14ac:dyDescent="0.3">
       <c r="A167" s="7" t="s">
         <v>585</v>
       </c>
@@ -10672,7 +10672,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="184" spans="1:2" ht="57" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A184" s="7" t="s">
         <v>618</v>
       </c>
@@ -10696,7 +10696,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="187" spans="1:2" ht="57" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A187" s="7" t="s">
         <v>604</v>
       </c>
@@ -10704,7 +10704,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="188" spans="1:2" ht="57" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A188" s="7" t="s">
         <v>605</v>
       </c>
@@ -10720,7 +10720,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="190" spans="1:2" ht="57" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A190" s="7" t="s">
         <v>607</v>
       </c>
@@ -10728,7 +10728,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="191" spans="1:2" ht="57" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A191" s="7" t="s">
         <v>608</v>
       </c>
@@ -10736,7 +10736,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="192" spans="1:2" ht="57" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A192" s="7" t="s">
         <v>609</v>
       </c>
@@ -10744,7 +10744,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="193" spans="1:2" ht="57" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A193" s="7" t="s">
         <v>610</v>
       </c>
@@ -10752,7 +10752,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="194" spans="1:2" ht="57" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A194" s="7" t="s">
         <v>611</v>
       </c>
@@ -10768,7 +10768,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="196" spans="1:2" ht="57" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A196" s="7" t="s">
         <v>613</v>
       </c>
@@ -10792,7 +10792,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="199" spans="1:2" ht="57" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A199" s="7" t="s">
         <v>616</v>
       </c>
@@ -10816,7 +10816,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="202" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A202" s="7" t="s">
         <v>621</v>
       </c>
@@ -10824,7 +10824,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="203" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:2" ht="34.200000000000003" x14ac:dyDescent="0.3">
       <c r="A203" s="8" t="s">
         <v>622</v>
       </c>
@@ -10848,7 +10848,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="206" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:2" ht="34.200000000000003" x14ac:dyDescent="0.3">
       <c r="A206" s="7" t="s">
         <v>625</v>
       </c>
@@ -10872,7 +10872,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="209" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:2" ht="34.200000000000003" x14ac:dyDescent="0.3">
       <c r="A209" s="7" t="s">
         <v>628</v>
       </c>
@@ -10880,7 +10880,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="210" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:2" ht="34.200000000000003" x14ac:dyDescent="0.3">
       <c r="A210" s="7" t="s">
         <v>629</v>
       </c>
@@ -10904,7 +10904,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="213" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:2" ht="34.200000000000003" x14ac:dyDescent="0.3">
       <c r="A213" s="7" t="s">
         <v>636</v>
       </c>
@@ -10912,7 +10912,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="214" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A214" s="7" t="s">
         <v>632</v>
       </c>
@@ -10920,7 +10920,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="215" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A215" s="7" t="s">
         <v>634</v>
       </c>
@@ -10928,7 +10928,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="216" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A216" s="7" t="s">
         <v>635</v>
       </c>
@@ -10944,7 +10944,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="218" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:2" ht="34.200000000000003" x14ac:dyDescent="0.3">
       <c r="A218" s="7" t="s">
         <v>637</v>
       </c>
@@ -10952,7 +10952,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="219" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:2" ht="34.200000000000003" x14ac:dyDescent="0.3">
       <c r="A219" s="7" t="s">
         <v>638</v>
       </c>
@@ -10960,7 +10960,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="220" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A220" s="7" t="s">
         <v>639</v>
       </c>
@@ -10984,7 +10984,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="223" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A223" s="7" t="s">
         <v>640</v>
       </c>
@@ -10992,7 +10992,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="224" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A224" s="7" t="s">
         <v>644</v>
       </c>
@@ -11008,7 +11008,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="226" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A226" s="7" t="s">
         <v>641</v>
       </c>
@@ -11024,7 +11024,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="228" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A228" s="7" t="s">
         <v>647</v>
       </c>
@@ -11032,7 +11032,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="229" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A229" s="7" t="s">
         <v>648</v>
       </c>
@@ -11040,7 +11040,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="230" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:2" ht="34.200000000000003" x14ac:dyDescent="0.3">
       <c r="A230" s="7" t="s">
         <v>649</v>
       </c>
@@ -11048,7 +11048,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="231" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A231" s="7" t="s">
         <v>650</v>
       </c>
@@ -11072,7 +11072,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="234" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A234" s="7" t="s">
         <v>653</v>
       </c>
@@ -11160,7 +11160,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="245" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A245" s="7" t="s">
         <v>664</v>
       </c>
@@ -11312,7 +11312,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="264" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A264" s="7" t="s">
         <v>681</v>
       </c>
@@ -11360,7 +11360,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="270" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A270" s="7" t="s">
         <v>689</v>
       </c>
@@ -11568,7 +11568,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="296" spans="1:2" ht="57" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A296" s="7" t="s">
         <v>717</v>
       </c>
@@ -11584,7 +11584,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="298" spans="1:2" ht="57" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A298" s="7" t="s">
         <v>715</v>
       </c>
@@ -11616,7 +11616,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="302" spans="1:2" ht="57" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A302" s="7" t="s">
         <v>720</v>
       </c>
@@ -11624,7 +11624,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="303" spans="1:2" ht="57" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A303" s="7" t="s">
         <v>721</v>
       </c>
@@ -11672,7 +11672,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="309" spans="1:2" ht="57" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A309" s="7" t="s">
         <v>727</v>
       </c>
@@ -11680,7 +11680,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="310" spans="1:2" ht="57" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A310" s="7" t="s">
         <v>728</v>
       </c>
@@ -11712,7 +11712,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="314" spans="1:2" ht="57" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A314" s="7" t="s">
         <v>732</v>
       </c>
@@ -11752,7 +11752,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="319" spans="1:2" ht="57" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A319" s="7" t="s">
         <v>737</v>
       </c>
@@ -11792,7 +11792,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="324" spans="1:2" ht="57" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A324" s="7" t="s">
         <v>742</v>
       </c>
@@ -11840,7 +11840,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="330" spans="1:2" ht="57" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A330" s="7" t="s">
         <v>1503</v>
       </c>
@@ -11864,7 +11864,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="333" spans="1:2" ht="57" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A333" s="7" t="s">
         <v>749</v>
       </c>
@@ -11872,7 +11872,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="334" spans="1:2" ht="57" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A334" s="7" t="s">
         <v>755</v>
       </c>
@@ -11880,7 +11880,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="335" spans="1:2" ht="57" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A335" s="7" t="s">
         <v>750</v>
       </c>
@@ -11888,7 +11888,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="336" spans="1:2" ht="57" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:2" ht="34.200000000000003" x14ac:dyDescent="0.3">
       <c r="A336" s="7" t="s">
         <v>751</v>
       </c>
@@ -11896,7 +11896,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="337" spans="1:2" ht="57" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A337" s="7" t="s">
         <v>756</v>
       </c>
@@ -12000,7 +12000,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="350" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A350" s="7" t="s">
         <v>767</v>
       </c>
@@ -12032,7 +12032,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="354" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A354" s="7" t="s">
         <v>771</v>
       </c>
@@ -12048,7 +12048,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="356" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:2" ht="34.200000000000003" x14ac:dyDescent="0.3">
       <c r="A356" s="7" t="s">
         <v>776</v>
       </c>
@@ -12056,7 +12056,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="357" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:2" ht="34.200000000000003" x14ac:dyDescent="0.3">
       <c r="A357" s="7" t="s">
         <v>772</v>
       </c>
@@ -12064,7 +12064,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="358" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A358" s="7" t="s">
         <v>773</v>
       </c>
@@ -12072,7 +12072,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="359" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A359" s="7" t="s">
         <v>774</v>
       </c>
@@ -12088,7 +12088,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="361" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A361" s="7" t="s">
         <v>778</v>
       </c>
@@ -12104,7 +12104,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="363" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A363" s="7" t="s">
         <v>780</v>
       </c>
@@ -12112,7 +12112,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="364" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A364" s="7" t="s">
         <v>781</v>
       </c>
@@ -12120,7 +12120,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="365" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:2" ht="34.200000000000003" x14ac:dyDescent="0.3">
       <c r="A365" s="7" t="s">
         <v>782</v>
       </c>
@@ -12128,7 +12128,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="366" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:2" ht="34.200000000000003" x14ac:dyDescent="0.3">
       <c r="A366" s="7" t="s">
         <v>783</v>
       </c>
@@ -12136,7 +12136,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="367" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:2" ht="34.200000000000003" x14ac:dyDescent="0.3">
       <c r="A367" s="7" t="s">
         <v>784</v>
       </c>
@@ -12144,7 +12144,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="368" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A368" s="7" t="s">
         <v>785</v>
       </c>
@@ -12152,7 +12152,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="369" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A369" s="7" t="s">
         <v>786</v>
       </c>
@@ -12160,7 +12160,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="370" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A370" s="7" t="s">
         <v>787</v>
       </c>
@@ -12168,7 +12168,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="371" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A371" s="7" t="s">
         <v>788</v>
       </c>
@@ -12176,7 +12176,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="372" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A372" s="7" t="s">
         <v>789</v>
       </c>
@@ -12184,7 +12184,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="373" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:2" ht="34.200000000000003" x14ac:dyDescent="0.3">
       <c r="A373" s="7" t="s">
         <v>790</v>
       </c>
@@ -12192,7 +12192,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="374" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A374" s="7" t="s">
         <v>791</v>
       </c>
@@ -12200,7 +12200,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="375" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:2" ht="34.200000000000003" x14ac:dyDescent="0.3">
       <c r="A375" s="7" t="s">
         <v>792</v>
       </c>
@@ -12208,7 +12208,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="376" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:2" ht="34.200000000000003" x14ac:dyDescent="0.3">
       <c r="A376" s="7" t="s">
         <v>793</v>
       </c>
@@ -12240,7 +12240,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="380" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:2" ht="34.200000000000003" x14ac:dyDescent="0.3">
       <c r="A380" s="7" t="s">
         <v>797</v>
       </c>
@@ -12248,7 +12248,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="381" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A381" s="7" t="s">
         <v>798</v>
       </c>
@@ -12264,7 +12264,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="383" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A383" s="7" t="s">
         <v>810</v>
       </c>
@@ -12288,7 +12288,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="386" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:2" ht="34.200000000000003" x14ac:dyDescent="0.3">
       <c r="A386" s="7" t="s">
         <v>801</v>
       </c>
@@ -12304,7 +12304,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="388" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A388" s="7" t="s">
         <v>803</v>
       </c>
@@ -12328,7 +12328,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="391" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A391" s="7" t="s">
         <v>806</v>
       </c>
@@ -12336,7 +12336,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="392" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:2" ht="34.200000000000003" x14ac:dyDescent="0.3">
       <c r="A392" s="7" t="s">
         <v>807</v>
       </c>
@@ -12352,7 +12352,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="394" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A394" s="7" t="s">
         <v>812</v>
       </c>
@@ -12360,7 +12360,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="395" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:2" ht="34.200000000000003" x14ac:dyDescent="0.3">
       <c r="A395" s="7" t="s">
         <v>811</v>
       </c>
@@ -12416,7 +12416,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="402" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A402" s="7" t="s">
         <v>1504</v>
       </c>
@@ -12472,7 +12472,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="409" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A409" s="7" t="s">
         <v>823</v>
       </c>
@@ -12568,7 +12568,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="421" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="421" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A421" s="7" t="s">
         <v>842</v>
       </c>
@@ -12640,7 +12640,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="430" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="430" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A430" s="7" t="s">
         <v>860</v>
       </c>
@@ -12656,7 +12656,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="432" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="432" spans="1:2" ht="34.200000000000003" x14ac:dyDescent="0.3">
       <c r="A432" s="7" t="s">
         <v>845</v>
       </c>
@@ -12664,7 +12664,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="433" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="433" spans="1:2" ht="34.200000000000003" x14ac:dyDescent="0.3">
       <c r="A433" s="7" t="s">
         <v>846</v>
       </c>
@@ -12680,7 +12680,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="435" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="435" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A435" s="7" t="s">
         <v>848</v>
       </c>
@@ -12688,7 +12688,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="436" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="436" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A436" s="7" t="s">
         <v>849</v>
       </c>
@@ -12696,7 +12696,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="437" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="437" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A437" s="7" t="s">
         <v>850</v>
       </c>
@@ -12712,7 +12712,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="439" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="439" spans="1:2" ht="34.200000000000003" x14ac:dyDescent="0.3">
       <c r="A439" s="7" t="s">
         <v>852</v>
       </c>
@@ -12728,7 +12728,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="441" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="441" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A441" s="7" t="s">
         <v>854</v>
       </c>
@@ -12736,7 +12736,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="442" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="442" spans="1:2" ht="34.200000000000003" x14ac:dyDescent="0.3">
       <c r="A442" s="7" t="s">
         <v>855</v>
       </c>
@@ -12760,7 +12760,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="445" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="445" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A445" s="7" t="s">
         <v>858</v>
       </c>
@@ -12872,7 +12872,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="459" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="459" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A459" s="7" t="s">
         <v>874</v>
       </c>
@@ -12880,7 +12880,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="460" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="460" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A460" s="7" t="s">
         <v>875</v>
       </c>
@@ -12912,7 +12912,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="464" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="464" spans="1:2" ht="34.200000000000003" x14ac:dyDescent="0.3">
       <c r="A464" s="7" t="s">
         <v>879</v>
       </c>
@@ -12920,7 +12920,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="465" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="465" spans="1:2" ht="34.200000000000003" x14ac:dyDescent="0.3">
       <c r="A465" s="7" t="s">
         <v>880</v>
       </c>
@@ -12968,7 +12968,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="471" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="471" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A471" s="7" t="s">
         <v>886</v>
       </c>
@@ -12984,7 +12984,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="473" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="473" spans="1:2" ht="34.200000000000003" x14ac:dyDescent="0.3">
       <c r="A473" s="7" t="s">
         <v>888</v>
       </c>
@@ -13024,7 +13024,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="478" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="478" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A478" s="7" t="s">
         <v>893</v>
       </c>
@@ -13032,7 +13032,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="479" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="479" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A479" s="7" t="s">
         <v>900</v>
       </c>
@@ -13056,7 +13056,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="482" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="482" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A482" s="7" t="s">
         <v>895</v>
       </c>
@@ -13064,7 +13064,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="483" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="483" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A483" s="7" t="s">
         <v>896</v>
       </c>
@@ -13104,7 +13104,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="488" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="488" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A488" s="7" t="s">
         <v>902</v>
       </c>
@@ -13160,7 +13160,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="495" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="495" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A495" s="7" t="s">
         <v>909</v>
       </c>
@@ -13176,7 +13176,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="497" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="497" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A497" s="7" t="s">
         <v>912</v>
       </c>
@@ -13368,7 +13368,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="521" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="521" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A521" s="7" t="s">
         <v>932</v>
       </c>
@@ -13376,7 +13376,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="522" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="522" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A522" s="7" t="s">
         <v>937</v>
       </c>
@@ -13637,7 +13637,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="555" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="555" spans="1:2" ht="34.200000000000003" x14ac:dyDescent="0.3">
       <c r="A555" s="7" t="s">
         <v>969</v>
       </c>
@@ -13645,7 +13645,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="556" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="556" spans="1:2" ht="34.200000000000003" x14ac:dyDescent="0.3">
       <c r="A556" s="7" t="s">
         <v>970</v>
       </c>
@@ -13653,7 +13653,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="557" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="557" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A557" s="7" t="s">
         <v>971</v>
       </c>
@@ -13661,7 +13661,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="558" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="558" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A558" s="7" t="s">
         <v>973</v>
       </c>
@@ -13685,7 +13685,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="561" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="561" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A561" s="7" t="s">
         <v>976</v>
       </c>
@@ -13693,7 +13693,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="562" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="562" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A562" s="7" t="s">
         <v>977</v>
       </c>
@@ -13701,7 +13701,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="563" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="563" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A563" s="7" t="s">
         <v>978</v>
       </c>
@@ -13725,7 +13725,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="566" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="566" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A566" s="7" t="s">
         <v>981</v>
       </c>
@@ -13733,7 +13733,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="567" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="567" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A567" s="7" t="s">
         <v>982</v>
       </c>
@@ -13741,7 +13741,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="568" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="568" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A568" s="7" t="s">
         <v>983</v>
       </c>
@@ -13773,7 +13773,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="572" spans="1:2" ht="57" x14ac:dyDescent="0.3">
+    <row r="572" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A572" s="7" t="s">
         <v>986</v>
       </c>
@@ -13781,7 +13781,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="573" spans="1:2" ht="57" x14ac:dyDescent="0.3">
+    <row r="573" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A573" s="7" t="s">
         <v>987</v>
       </c>
@@ -13789,7 +13789,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="574" spans="1:2" ht="57" x14ac:dyDescent="0.3">
+    <row r="574" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A574" s="7" t="s">
         <v>988</v>
       </c>
@@ -13821,7 +13821,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="578" spans="1:2" ht="57" x14ac:dyDescent="0.3">
+    <row r="578" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A578" s="7" t="s">
         <v>1010</v>
       </c>
@@ -13829,7 +13829,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="579" spans="1:2" ht="57" x14ac:dyDescent="0.3">
+    <row r="579" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A579" s="7" t="s">
         <v>993</v>
       </c>
@@ -13837,7 +13837,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="580" spans="1:2" ht="57" x14ac:dyDescent="0.3">
+    <row r="580" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A580" s="7" t="s">
         <v>994</v>
       </c>
@@ -13909,7 +13909,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="589" spans="1:2" ht="57" x14ac:dyDescent="0.3">
+    <row r="589" spans="1:2" ht="34.200000000000003" x14ac:dyDescent="0.3">
       <c r="A589" s="7" t="s">
         <v>1003</v>
       </c>
@@ -13917,7 +13917,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="590" spans="1:2" ht="57" x14ac:dyDescent="0.3">
+    <row r="590" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A590" s="7" t="s">
         <v>1004</v>
       </c>
@@ -13925,7 +13925,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="591" spans="1:2" ht="57" x14ac:dyDescent="0.3">
+    <row r="591" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A591" s="7" t="s">
         <v>1005</v>
       </c>
@@ -13933,7 +13933,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="592" spans="1:2" ht="57" x14ac:dyDescent="0.3">
+    <row r="592" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A592" s="7" t="s">
         <v>1006</v>
       </c>
@@ -13941,7 +13941,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="593" spans="1:2" ht="57" x14ac:dyDescent="0.3">
+    <row r="593" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A593" s="7" t="s">
         <v>1007</v>
       </c>
@@ -13981,7 +13981,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="598" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="598" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A598" s="7" t="s">
         <v>1020</v>
       </c>
@@ -14037,7 +14037,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="605" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="605" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A605" s="7" t="s">
         <v>1018</v>
       </c>
@@ -14045,7 +14045,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="606" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="606" spans="1:2" ht="34.200000000000003" x14ac:dyDescent="0.3">
       <c r="A606" s="7" t="s">
         <v>1037</v>
       </c>
@@ -14053,7 +14053,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="607" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="607" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A607" s="7" t="s">
         <v>1021</v>
       </c>
@@ -14061,7 +14061,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="608" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="608" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A608" s="7" t="s">
         <v>1022</v>
       </c>
@@ -14069,7 +14069,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="609" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="609" spans="1:2" ht="34.200000000000003" x14ac:dyDescent="0.3">
       <c r="A609" s="7" t="s">
         <v>1023</v>
       </c>
@@ -14077,7 +14077,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="610" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="610" spans="1:2" ht="34.200000000000003" x14ac:dyDescent="0.3">
       <c r="A610" s="7" t="s">
         <v>1024</v>
       </c>
@@ -14101,7 +14101,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="613" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="613" spans="1:2" ht="34.200000000000003" x14ac:dyDescent="0.3">
       <c r="A613" s="7" t="s">
         <v>1027</v>
       </c>
@@ -14109,7 +14109,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="614" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="614" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A614" s="7" t="s">
         <v>1028</v>
       </c>
@@ -14117,7 +14117,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="615" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="615" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A615" s="7" t="s">
         <v>1029</v>
       </c>
@@ -14125,7 +14125,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="616" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="616" spans="1:2" ht="34.200000000000003" x14ac:dyDescent="0.3">
       <c r="A616" s="7" t="s">
         <v>1036</v>
       </c>
@@ -14157,7 +14157,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="620" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="620" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A620" s="7" t="s">
         <v>1033</v>
       </c>
@@ -14173,7 +14173,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="622" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="622" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A622" s="7" t="s">
         <v>1035</v>
       </c>
@@ -14189,7 +14189,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="624" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="624" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A624" s="7" t="s">
         <v>1038</v>
       </c>
@@ -14197,7 +14197,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="625" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="625" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A625" s="7" t="s">
         <v>1039</v>
       </c>
@@ -14205,7 +14205,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="626" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="626" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A626" s="7" t="s">
         <v>1055</v>
       </c>
@@ -14229,7 +14229,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="629" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="629" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A629" s="7" t="s">
         <v>1043</v>
       </c>
@@ -14237,7 +14237,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="630" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="630" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A630" s="7" t="s">
         <v>1044</v>
       </c>
@@ -14253,7 +14253,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="632" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="632" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A632" s="7" t="s">
         <v>1045</v>
       </c>
@@ -14261,7 +14261,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="633" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="633" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A633" s="7" t="s">
         <v>1057</v>
       </c>
@@ -14285,7 +14285,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="636" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="636" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A636" s="7" t="s">
         <v>1047</v>
       </c>
@@ -14317,7 +14317,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="640" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="640" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A640" s="7" t="s">
         <v>1051</v>
       </c>
@@ -14381,7 +14381,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="648" spans="1:2" ht="57" x14ac:dyDescent="0.3">
+    <row r="648" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A648" s="7" t="s">
         <v>1061</v>
       </c>
@@ -14389,7 +14389,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="649" spans="1:2" ht="57" x14ac:dyDescent="0.3">
+    <row r="649" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A649" s="7" t="s">
         <v>1062</v>
       </c>
@@ -14413,7 +14413,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="652" spans="1:2" ht="57" x14ac:dyDescent="0.3">
+    <row r="652" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A652" s="7" t="s">
         <v>1065</v>
       </c>
@@ -14421,7 +14421,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="653" spans="1:2" ht="57" x14ac:dyDescent="0.3">
+    <row r="653" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A653" s="7" t="s">
         <v>1066</v>
       </c>
@@ -14429,7 +14429,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="654" spans="1:2" ht="57" x14ac:dyDescent="0.3">
+    <row r="654" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A654" s="7" t="s">
         <v>1067</v>
       </c>
@@ -14437,7 +14437,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="655" spans="1:2" ht="57" x14ac:dyDescent="0.3">
+    <row r="655" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A655" s="7" t="s">
         <v>1068</v>
       </c>
@@ -14453,7 +14453,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="657" spans="1:2" ht="57" x14ac:dyDescent="0.3">
+    <row r="657" spans="1:2" ht="34.200000000000003" x14ac:dyDescent="0.3">
       <c r="A657" s="7" t="s">
         <v>1070</v>
       </c>
@@ -14501,7 +14501,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="663" spans="1:2" ht="57" x14ac:dyDescent="0.3">
+    <row r="663" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A663" s="7" t="s">
         <v>1076</v>
       </c>
@@ -14701,7 +14701,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="688" spans="1:2" ht="57" x14ac:dyDescent="0.3">
+    <row r="688" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A688" s="7" t="s">
         <v>1102</v>
       </c>
@@ -14709,7 +14709,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="689" spans="1:2" ht="57" x14ac:dyDescent="0.3">
+    <row r="689" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A689" s="7" t="s">
         <v>1103</v>
       </c>
@@ -14741,7 +14741,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="693" spans="1:2" ht="57" x14ac:dyDescent="0.3">
+    <row r="693" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A693" s="7" t="s">
         <v>1110</v>
       </c>
@@ -14749,7 +14749,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="694" spans="1:2" ht="57" x14ac:dyDescent="0.3">
+    <row r="694" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A694" s="7" t="s">
         <v>1106</v>
       </c>
@@ -14765,7 +14765,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="696" spans="1:2" ht="57" x14ac:dyDescent="0.3">
+    <row r="696" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A696" s="7" t="s">
         <v>1108</v>
       </c>
@@ -14861,7 +14861,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="709" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="709" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A709" s="7" t="s">
         <v>1122</v>
       </c>
@@ -14877,7 +14877,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="711" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="711" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A711" s="7" t="s">
         <v>1124</v>
       </c>
@@ -14885,7 +14885,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="712" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="712" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A712" s="7" t="s">
         <v>1125</v>
       </c>
@@ -14901,7 +14901,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="714" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="714" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A714" s="7" t="s">
         <v>1127</v>
       </c>
@@ -14909,7 +14909,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="715" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="715" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A715" s="7" t="s">
         <v>1128</v>
       </c>
@@ -14917,7 +14917,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="716" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="716" spans="1:2" ht="34.200000000000003" x14ac:dyDescent="0.3">
       <c r="A716" s="7" t="s">
         <v>1129</v>
       </c>
@@ -14957,7 +14957,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="721" spans="1:2" ht="57" x14ac:dyDescent="0.3">
+    <row r="721" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A721" s="7" t="s">
         <v>1507</v>
       </c>
@@ -14987,7 +14987,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="725" spans="1:2" ht="57" x14ac:dyDescent="0.3">
+    <row r="725" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A725" s="7" t="s">
         <v>1508</v>
       </c>
@@ -15003,7 +15003,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="727" spans="1:2" ht="57" x14ac:dyDescent="0.3">
+    <row r="727" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A727" s="7" t="s">
         <v>1137</v>
       </c>
@@ -15043,7 +15043,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="732" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="732" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A732" s="7" t="s">
         <v>1148</v>
       </c>
@@ -15051,7 +15051,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="733" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="733" spans="1:2" ht="34.200000000000003" x14ac:dyDescent="0.3">
       <c r="A733" s="7" t="s">
         <v>1149</v>
       </c>
@@ -15083,7 +15083,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="737" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="737" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A737" s="7" t="s">
         <v>1153</v>
       </c>
@@ -15091,7 +15091,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="738" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="738" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A738" s="7" t="s">
         <v>1154</v>
       </c>
@@ -15123,7 +15123,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="742" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="742" spans="1:2" ht="34.200000000000003" x14ac:dyDescent="0.3">
       <c r="A742" s="7" t="s">
         <v>1158</v>
       </c>
@@ -15131,7 +15131,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="743" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="743" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A743" s="8" t="s">
         <v>1159</v>
       </c>
@@ -15139,7 +15139,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="744" spans="1:2" ht="45.6" x14ac:dyDescent="0.3">
+    <row r="744" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A744" s="7" t="s">
         <v>1160</v>
       </c>
@@ -15355,7 +15355,7 @@
         <v>1144</v>
       </c>
     </row>
-    <row r="771" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="771" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A771" s="7" t="s">
         <v>1176</v>
       </c>
@@ -15363,7 +15363,7 @@
         <v>1144</v>
       </c>
     </row>
-    <row r="772" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="772" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A772" s="7" t="s">
         <v>1179</v>
       </c>
@@ -15371,7 +15371,7 @@
         <v>1144</v>
       </c>
     </row>
-    <row r="773" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="773" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A773" s="7" t="s">
         <v>1177</v>
       </c>
@@ -15411,7 +15411,7 @@
         <v>1144</v>
       </c>
     </row>
-    <row r="778" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="778" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A778" s="7" t="s">
         <v>1185</v>
       </c>
@@ -15499,7 +15499,7 @@
         <v>1144</v>
       </c>
     </row>
-    <row r="789" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="789" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A789" s="7" t="s">
         <v>1190</v>
       </c>
@@ -15672,7 +15672,7 @@
         <v>1144</v>
       </c>
     </row>
-    <row r="811" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="811" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A811" s="9" t="s">
         <v>1216</v>
       </c>
@@ -15728,7 +15728,7 @@
         <v>1144</v>
       </c>
     </row>
-    <row r="818" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="818" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A818" s="9" t="s">
         <v>1211</v>
       </c>
@@ -15800,7 +15800,7 @@
         <v>1144</v>
       </c>
     </row>
-    <row r="827" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="827" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A827" s="9" t="s">
         <v>1242</v>
       </c>
@@ -15824,7 +15824,7 @@
         <v>1144</v>
       </c>
     </row>
-    <row r="830" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="830" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A830" s="9" t="s">
         <v>1245</v>
       </c>
@@ -15840,7 +15840,7 @@
         <v>1144</v>
       </c>
     </row>
-    <row r="832" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="832" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A832" s="8" t="s">
         <v>1243</v>
       </c>
@@ -15888,7 +15888,7 @@
         <v>1144</v>
       </c>
     </row>
-    <row r="838" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="838" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A838" s="9" t="s">
         <v>1233</v>
       </c>
@@ -15920,7 +15920,7 @@
         <v>1144</v>
       </c>
     </row>
-    <row r="842" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="842" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A842" s="9" t="s">
         <v>1237</v>
       </c>
@@ -16232,7 +16232,7 @@
         <v>1144</v>
       </c>
     </row>
-    <row r="881" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="881" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A881" s="9" t="s">
         <v>1260</v>
       </c>
@@ -16248,7 +16248,7 @@
         <v>1144</v>
       </c>
     </row>
-    <row r="883" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="883" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A883" s="9" t="s">
         <v>1346</v>
       </c>
@@ -16296,7 +16296,7 @@
         <v>1144</v>
       </c>
     </row>
-    <row r="889" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="889" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A889" s="9" t="s">
         <v>1351</v>
       </c>
@@ -16368,7 +16368,7 @@
         <v>1144</v>
       </c>
     </row>
-    <row r="898" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="898" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A898" s="9" t="s">
         <v>1524</v>
       </c>
@@ -16400,7 +16400,7 @@
         <v>1144</v>
       </c>
     </row>
-    <row r="902" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="902" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A902" s="9" t="s">
         <v>1270</v>
       </c>
@@ -16424,7 +16424,7 @@
         <v>1144</v>
       </c>
     </row>
-    <row r="905" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="905" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A905" s="9" t="s">
         <v>1355</v>
       </c>
@@ -16440,7 +16440,7 @@
         <v>1144</v>
       </c>
     </row>
-    <row r="907" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="907" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A907" s="9" t="s">
         <v>1273</v>
       </c>
@@ -16464,7 +16464,7 @@
         <v>1144</v>
       </c>
     </row>
-    <row r="910" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="910" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A910" s="9" t="s">
         <v>1357</v>
       </c>
@@ -16480,7 +16480,7 @@
         <v>1144</v>
       </c>
     </row>
-    <row r="912" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="912" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A912" s="9" t="s">
         <v>1527</v>
       </c>
@@ -16624,7 +16624,7 @@
         <v>1144</v>
       </c>
     </row>
-    <row r="930" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="930" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A930" s="9" t="s">
         <v>1367</v>
       </c>
@@ -16728,7 +16728,7 @@
         <v>1144</v>
       </c>
     </row>
-    <row r="943" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="943" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A943" s="9" t="s">
         <v>1376</v>
       </c>
@@ -16784,7 +16784,7 @@
         <v>1144</v>
       </c>
     </row>
-    <row r="950" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="950" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A950" s="9" t="s">
         <v>1378</v>
       </c>
@@ -16792,7 +16792,7 @@
         <v>1144</v>
       </c>
     </row>
-    <row r="951" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="951" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A951" s="9" t="s">
         <v>1380</v>
       </c>
@@ -16936,7 +16936,7 @@
         <v>1144</v>
       </c>
     </row>
-    <row r="969" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="969" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A969" s="9" t="s">
         <v>1308</v>
       </c>
@@ -16992,7 +16992,7 @@
         <v>1144</v>
       </c>
     </row>
-    <row r="976" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="976" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A976" s="9" t="s">
         <v>1312</v>
       </c>
@@ -17016,7 +17016,7 @@
         <v>1144</v>
       </c>
     </row>
-    <row r="979" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="979" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A979" s="9" t="s">
         <v>1315</v>
       </c>
@@ -17208,7 +17208,7 @@
         <v>1144</v>
       </c>
     </row>
-    <row r="1003" spans="1:2" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="1003" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1003" s="9" t="s">
         <v>1391</v>
       </c>

</xml_diff>